<commit_message>
commiting batch module valid data end to end
</commit_message>
<xml_diff>
--- a/Team12_APIExplorers_LMS_Hackathon_Mar2024/src/test/resources/testdata.xlsx
+++ b/Team12_APIExplorers_LMS_Hackathon_Mar2024/src/test/resources/testdata.xlsx
@@ -5,20 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudha\eclipse-workspace\Team12_APIExplorers_LMS_Hackathon_Mar2024\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13313\git\Team12_APIExplorers_LMS_Hackathon_Mar2024\Team12_APIExplorers_LMS_Hackathon_Mar2024\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C495E9CB-EB8C-4381-B560-D3FAA9870CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F97DC51-0F02-46AC-95AA-171B3564288D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="API_Authentication" sheetId="1" r:id="rId1"/>
     <sheet name="UserLoginController" sheetId="2" r:id="rId2"/>
     <sheet name="ProgramModule" sheetId="3" r:id="rId3"/>
-    <sheet name="ProgramBatchModule" sheetId="4" r:id="rId4"/>
-    <sheet name="UserModule" sheetId="5" r:id="rId5"/>
-    <sheet name="RoleMapController" sheetId="6" r:id="rId6"/>
+    <sheet name="BatchPostdata" sheetId="4" r:id="rId4"/>
+    <sheet name="BatchUpdateData" sheetId="7" r:id="rId5"/>
+    <sheet name="UserModule" sheetId="5" r:id="rId6"/>
+    <sheet name="RoleMapController" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>password</t>
   </si>
@@ -42,13 +43,43 @@
   </si>
   <si>
     <t>userLoginEmailid</t>
+  </si>
+  <si>
+    <t>batchDescription</t>
+  </si>
+  <si>
+    <t>batchName</t>
+  </si>
+  <si>
+    <t>batchNoOfClasses</t>
+  </si>
+  <si>
+    <t>batchStatus</t>
+  </si>
+  <si>
+    <t>programId</t>
+  </si>
+  <si>
+    <t>Selenium with java</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>programName</t>
+  </si>
+  <si>
+    <t>March24-APIGurus-SDET-541</t>
+  </si>
+  <si>
+    <t>SDETQA9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,6 +100,12 @@
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -92,10 +129,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -379,7 +417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -436,19 +474,125 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E31ECA9-8463-4522-A80D-EFD48E5DAC44}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>16378</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02FEB0FE-52DC-45FD-B8EB-2792A4851CA7}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>16378</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A047755E-F8A5-4220-8202-E93EC965FB77}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -460,7 +604,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A34CDEC-A329-4AEA-99E0-2070FF6F4FD7}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
commiting login post program post and all valid data requests in flow
</commit_message>
<xml_diff>
--- a/Team12_APIExplorers_LMS_Hackathon_Mar2024/src/test/resources/testdata.xlsx
+++ b/Team12_APIExplorers_LMS_Hackathon_Mar2024/src/test/resources/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13313\git\Team12_APIExplorers_LMS_Hackathon_Mar2024\Team12_APIExplorers_LMS_Hackathon_Mar2024\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F97DC51-0F02-46AC-95AA-171B3564288D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61293708-83F8-469C-B8FD-4DD02895368D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>password</t>
   </si>
@@ -69,10 +69,25 @@
     <t>programName</t>
   </si>
   <si>
-    <t>March24-APIGurus-SDET-541</t>
-  </si>
-  <si>
-    <t>SDETQA9</t>
+    <t>programDescription</t>
+  </si>
+  <si>
+    <t>programStatus</t>
+  </si>
+  <si>
+    <t>started</t>
+  </si>
+  <si>
+    <t>API_RestAssured</t>
+  </si>
+  <si>
+    <t>SDETQA12</t>
+  </si>
+  <si>
+    <t>API8</t>
+  </si>
+  <si>
+    <t>SDETQA21</t>
   </si>
 </sst>
 </file>
@@ -131,9 +146,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -418,24 +433,28 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -462,12 +481,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C1F7F9-21BC-4D4E-B2D2-8600B75F677C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -477,7 +526,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,37 +539,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>30</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2">
-        <v>16378</v>
       </c>
     </row>
   </sheetData>
@@ -547,22 +591,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -571,7 +615,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>25</v>
@@ -583,7 +627,7 @@
         <v>16378</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All running code with one bug
</commit_message>
<xml_diff>
--- a/Team12_APIExplorers_LMS_Hackathon_Mar2024/src/test/resources/testdata.xlsx
+++ b/Team12_APIExplorers_LMS_Hackathon_Mar2024/src/test/resources/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudha\git\Team12_APIExplorers_LMS_Hackathon_Mar2024\Team12_APIExplorers_LMS_Hackathon_Mar2024\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirti\git\Team12_APIExplorers_LMS_Hackathon_Mar2024\Team12_APIExplorers_LMS_Hackathon_Mar2024\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF68D99-A218-44D9-998D-4FEE92F7677B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6AF41E-6663-4FF9-80A0-BE495BB968C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="API_Authentication" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t>password</t>
   </si>
@@ -42,6 +42,39 @@
   </si>
   <si>
     <t>userLoginEmailid</t>
+  </si>
+  <si>
+    <t>ProgramName</t>
+  </si>
+  <si>
+    <t>ProgramStatus</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>ProgramDescription</t>
+  </si>
+  <si>
+    <t>This is test</t>
+  </si>
+  <si>
+    <t>This is update test</t>
+  </si>
+  <si>
+    <t>This is prgm name update test</t>
+  </si>
+  <si>
+    <t>1Java</t>
+  </si>
+  <si>
+    <t>1this is test</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>Javaal</t>
   </si>
 </sst>
 </file>
@@ -379,13 +412,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -393,7 +426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -416,7 +449,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -424,12 +457,130 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C1F7F9-21BC-4D4E-B2D2-8600B75F677C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -442,7 +593,7 @@
       <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -454,7 +605,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -468,7 +619,7 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Login Program User and RoleMap merge
</commit_message>
<xml_diff>
--- a/Team12_APIExplorers_LMS_Hackathon_Mar2024/src/test/resources/testdata.xlsx
+++ b/Team12_APIExplorers_LMS_Hackathon_Mar2024/src/test/resources/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudha\git\Team12_APIExplorers_LMS_Hackathon_Mar2024\Team12_APIExplorers_LMS_Hackathon_Mar2024\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF68D99-A218-44D9-998D-4FEE92F7677B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C81197-AE76-4D04-8530-3C39D48B22D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="API_Authentication" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="ProgramModule" sheetId="3" r:id="rId3"/>
     <sheet name="ProgramBatchModule" sheetId="4" r:id="rId4"/>
     <sheet name="UserModule" sheetId="5" r:id="rId5"/>
-    <sheet name="RoleMapController" sheetId="6" r:id="rId6"/>
+    <sheet name="UserUpdateRoleStatus" sheetId="7" r:id="rId6"/>
+    <sheet name="RoleMapController" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="95">
   <si>
     <t>password</t>
   </si>
@@ -42,13 +43,286 @@
   </si>
   <si>
     <t>userLoginEmailid</t>
+  </si>
+  <si>
+    <t>team1234</t>
+  </si>
+  <si>
+    <t>team12</t>
+  </si>
+  <si>
+    <t>userComments</t>
+  </si>
+  <si>
+    <t>userEduPg</t>
+  </si>
+  <si>
+    <t>userEduUg</t>
+  </si>
+  <si>
+    <t>userFirstName</t>
+  </si>
+  <si>
+    <t>userLastName</t>
+  </si>
+  <si>
+    <t>userLinkedinUrl</t>
+  </si>
+  <si>
+    <t>userLocation</t>
+  </si>
+  <si>
+    <t>loginStatus</t>
+  </si>
+  <si>
+    <t>userLoginEmail</t>
+  </si>
+  <si>
+    <t>userMiddleName</t>
+  </si>
+  <si>
+    <t>userPhoneNumber</t>
+  </si>
+  <si>
+    <t>roleId</t>
+  </si>
+  <si>
+    <t>userRoleStatus</t>
+  </si>
+  <si>
+    <t>userTimeZone</t>
+  </si>
+  <si>
+    <t>userVisaStatus</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>R03</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>InActive</t>
+  </si>
+  <si>
+    <t>Not-Specified</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>GC-EAD</t>
+  </si>
+  <si>
+    <t>H4-EAD</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>H1B</t>
+  </si>
+  <si>
+    <t>Canada-EAD</t>
+  </si>
+  <si>
+    <t>US-Citizen</t>
+  </si>
+  <si>
+    <t>Indian-Citizen</t>
+  </si>
+  <si>
+    <t>Canada-Citizen</t>
+  </si>
+  <si>
+    <t>PST</t>
+  </si>
+  <si>
+    <t>MST</t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>EST</t>
+  </si>
+  <si>
+    <t>IST</t>
+  </si>
+  <si>
+    <t>2team12@email.com</t>
+  </si>
+  <si>
+    <t>3team12@email.com</t>
+  </si>
+  <si>
+    <t>4team12@email.com</t>
+  </si>
+  <si>
+    <t>5team12@email.com</t>
+  </si>
+  <si>
+    <t>6team12@email.com</t>
+  </si>
+  <si>
+    <t>New user for Admin role</t>
+  </si>
+  <si>
+    <t>New user for Staff role</t>
+  </si>
+  <si>
+    <t>New user for Student role</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>sudha</t>
+  </si>
+  <si>
+    <t>debalina</t>
+  </si>
+  <si>
+    <t>archana</t>
+  </si>
+  <si>
+    <t>manali</t>
+  </si>
+  <si>
+    <t>sandhya</t>
+  </si>
+  <si>
+    <t>bhuvaneswari</t>
+  </si>
+  <si>
+    <t>sample1</t>
+  </si>
+  <si>
+    <t>sample2</t>
+  </si>
+  <si>
+    <t>sample3</t>
+  </si>
+  <si>
+    <t>sample4</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/test2</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/test3</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/test4</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/test5</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/test6</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/test7</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/test8</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/test9</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/test10</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>7team12@email.com</t>
+  </si>
+  <si>
+    <t>8team12@email.com</t>
+  </si>
+  <si>
+    <t>9team12@email.com</t>
+  </si>
+  <si>
+    <t>10team12@email.com</t>
+  </si>
+  <si>
+    <t>update user Location for Admin role</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>middle</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/apiexplorers</t>
+  </si>
+  <si>
+    <t>last</t>
+  </si>
+  <si>
+    <t>sudha@gmail.com</t>
+  </si>
+  <si>
+    <t>midle</t>
+  </si>
+  <si>
+    <t>lastt</t>
+  </si>
+  <si>
+    <t>invalidAdminId</t>
+  </si>
+  <si>
+    <t>ProgramName</t>
+  </si>
+  <si>
+    <t>ProgramStatus</t>
+  </si>
+  <si>
+    <t>ProgramDescription</t>
+  </si>
+  <si>
+    <t>This is test</t>
+  </si>
+  <si>
+    <t>This is update test</t>
+  </si>
+  <si>
+    <t>This is prgm name update test</t>
+  </si>
+  <si>
+    <t>1Java</t>
+  </si>
+  <si>
+    <t>1this is test</t>
+  </si>
+  <si>
+    <t>Javaao</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +344,23 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -79,7 +370,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -87,19 +378,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{7BC2183A-F2B9-469D-9809-E7403BE58932}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -377,15 +690,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -393,18 +706,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{FF015305-9BBF-44A4-884C-048487254FD3}"/>
     <hyperlink ref="A2" r:id="rId2" xr:uid="{6E2494EF-9FAD-4D7B-B581-7536C1F4EBE0}"/>
+    <hyperlink ref="A3" r:id="rId3" display="team12@gmail.com" xr:uid="{ACF6DB4E-72DC-4980-8275-399C6A651DC1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -416,7 +738,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -424,12 +746,130 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C1F7F9-21BC-4D4E-B2D2-8600B75F677C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -442,7 +882,7 @@
       <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -450,26 +890,708 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A047755E-F8A5-4220-8202-E93EC965FB77}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="24.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K2" t="s">
+        <v>79</v>
+      </c>
+      <c r="L2">
+        <v>8978518063</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L3">
+        <v>8978518064</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L4">
+        <v>1517181020</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" t="s">
+        <v>79</v>
+      </c>
+      <c r="L5">
+        <v>2122232425</v>
+      </c>
+      <c r="M5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" t="s">
+        <v>79</v>
+      </c>
+      <c r="L6">
+        <v>2627282930</v>
+      </c>
+      <c r="M6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L7">
+        <v>3323334353</v>
+      </c>
+      <c r="M7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O7" t="s">
+        <v>39</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8" t="s">
+        <v>79</v>
+      </c>
+      <c r="L8">
+        <v>3637383040</v>
+      </c>
+      <c r="M8" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O8" t="s">
+        <v>39</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" t="s">
+        <v>78</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K9" t="s">
+        <v>79</v>
+      </c>
+      <c r="L9">
+        <v>4142434445</v>
+      </c>
+      <c r="M9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" t="s">
+        <v>25</v>
+      </c>
+      <c r="O9" t="s">
+        <v>39</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" t="s">
+        <v>79</v>
+      </c>
+      <c r="L10">
+        <v>4647484950</v>
+      </c>
+      <c r="M10" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O10" t="s">
+        <v>39</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" t="s">
+        <v>72</v>
+      </c>
+      <c r="I11" t="s">
+        <v>78</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K11" t="s">
+        <v>79</v>
+      </c>
+      <c r="L11">
+        <v>5152535455</v>
+      </c>
+      <c r="M11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" t="s">
+        <v>25</v>
+      </c>
+      <c r="O11" t="s">
+        <v>39</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K12" t="s">
+        <v>79</v>
+      </c>
+      <c r="L12">
+        <v>4647484950</v>
+      </c>
+      <c r="M12" t="s">
+        <v>21</v>
+      </c>
+      <c r="N12" t="s">
+        <v>24</v>
+      </c>
+      <c r="O12" t="s">
+        <v>39</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="M13" t="s">
+        <v>23</v>
+      </c>
+      <c r="P13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{9EC109B1-C25E-4B73-9C65-DF69840CE3E8}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{35FAC877-EFE4-4342-B0F5-CD03E1FADB13}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{4048BD8F-5F11-4AAA-A73A-CA4CA08B4231}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{9B887EC8-52B4-4A66-9717-3ABF5671EB26}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{B0A544C3-D5AC-4E81-8362-361A455170EE}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{3280756A-6FA6-4FB2-87F0-6CEF4E38D1C3}"/>
+    <hyperlink ref="F3" r:id="rId7" xr:uid="{037FE3A7-703E-43E8-A677-4DF65D7209BA}"/>
+    <hyperlink ref="F4" r:id="rId8" xr:uid="{C1F7611D-59AB-434E-8129-E9FDCCD57ED4}"/>
+    <hyperlink ref="F5" r:id="rId9" xr:uid="{B36B5EE3-2279-45B0-835E-921E6BE9FD48}"/>
+    <hyperlink ref="F6" r:id="rId10" xr:uid="{C7ADF2E0-493E-4D3E-8856-24429AE76AA5}"/>
+    <hyperlink ref="F7" r:id="rId11" xr:uid="{5222DA66-0E3E-4FC9-B6F8-5C71241C7E87}"/>
+    <hyperlink ref="F8" r:id="rId12" xr:uid="{9E3057AE-CA26-4BFB-B3E1-DDF0F3BD54E1}"/>
+    <hyperlink ref="F9" r:id="rId13" xr:uid="{FAC1368D-613C-4838-9F7A-48091C82354C}"/>
+    <hyperlink ref="F10" r:id="rId14" xr:uid="{E03E1841-72C3-4A86-9C33-7BDDEBE7DDD4}"/>
+    <hyperlink ref="F11" r:id="rId15" xr:uid="{FFC48B3A-64F9-45F6-B49C-112ACAB6EE25}"/>
+    <hyperlink ref="J8" r:id="rId16" xr:uid="{F58CFCD8-2503-4CC1-9A98-E34666744986}"/>
+    <hyperlink ref="J9" r:id="rId17" xr:uid="{A109764A-2239-464A-9773-8419290B17CB}"/>
+    <hyperlink ref="J10" r:id="rId18" xr:uid="{AE95EA12-9638-4E9A-A5AF-C9FA4BAA25B1}"/>
+    <hyperlink ref="J11" r:id="rId19" xr:uid="{0F674B93-9C9B-4460-9482-4463479DFAD6}"/>
+    <hyperlink ref="F12" r:id="rId20" xr:uid="{7BED6C7B-C2FF-4AF9-9F64-D098A704CB2C}"/>
+    <hyperlink ref="J12" r:id="rId21" xr:uid="{F52A1E63-CADB-4C32-A542-17CEF759BEA4}"/>
+    <hyperlink ref="F2" r:id="rId22" xr:uid="{92EFB2C6-F142-451D-A2B0-F47CF0AD38EF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A34CDEC-A329-4AEA-99E0-2070FF6F4FD7}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A553D97-FF67-44F0-9D7E-2DC4C2AFC9B1}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A34CDEC-A329-4AEA-99E0-2070FF6F4FD7}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
+        <v>1234</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>